<commit_message>
Agregue reporte de egresos e ingresos
</commit_message>
<xml_diff>
--- a/requerimientos_sistema_salon_belleza_orden.xlsx
+++ b/requerimientos_sistema_salon_belleza_orden.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppEiker\SALON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppEiker\.Net\Git2\SALON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60F6759-9212-4305-91CA-B1532BF0E5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB58DF3-E70C-42EE-8388-99302B7E5B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Módulo</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>EN PROCESO</t>
+  </si>
+  <si>
+    <t>SIN INICIAR</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,15 +592,15 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
-        <v>34</v>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -606,14 +609,16 @@
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -621,14 +626,16 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -636,14 +643,16 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -651,14 +660,16 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -666,14 +677,16 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -688,7 +701,9 @@
         <v>25</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -696,14 +711,16 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -711,14 +728,16 @@
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -733,7 +752,9 @@
         <v>28</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -748,7 +769,9 @@
         <v>29</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -763,7 +786,9 @@
         <v>30</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -778,7 +803,9 @@
         <v>31</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -786,14 +813,16 @@
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>

</xml_diff>